<commit_message>
Fixed confirming and rejecting reports by supervisor Added BOT_NAME variable into .env
</commit_message>
<xml_diff>
--- a/schedule_sample.xlsx
+++ b/schedule_sample.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06.11.2024</t>
+          <t>15.11.2024</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>07.11.2024</t>
+          <t>16.11.2024</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>08.11.2024</t>
+          <t>17.11.2024</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>09.11.2024</t>
+          <t>18.11.2024</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10.11.2024</t>
+          <t>19.11.2024</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11.11.2024</t>
+          <t>20.11.2024</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>12.11.2024</t>
+          <t>21.11.2024</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13.11.2024</t>
+          <t>22.11.2024</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14.11.2024</t>
+          <t>23.11.2024</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15.11.2024</t>
+          <t>24.11.2024</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16.11.2024</t>
+          <t>25.11.2024</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17.11.2024</t>
+          <t>26.11.2024</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>18.11.2024</t>
+          <t>27.11.2024</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>19.11.2024</t>
+          <t>28.11.2024</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>20.11.2024</t>
+          <t>29.11.2024</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21.11.2024</t>
+          <t>30.11.2024</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>22.11.2024</t>
+          <t>01.12.2024</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23.11.2024</t>
+          <t>02.12.2024</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>24.11.2024</t>
+          <t>03.12.2024</t>
         </is>
       </c>
     </row>

</xml_diff>